<commit_message>
added geojson and started leaflet coding
</commit_message>
<xml_diff>
--- a/assets/priprecinct/house/ALL_uncontested_house.xlsx
+++ b/assets/priprecinct/house/ALL_uncontested_house.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="680" windowWidth="21320" windowHeight="13960" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="180" yWindow="700" windowWidth="19500" windowHeight="13960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="by-party" sheetId="3" r:id="rId1"/>
-    <sheet name="by-name" sheetId="7" r:id="rId2"/>
-    <sheet name="ALL_uncontested" sheetId="1" r:id="rId3"/>
+    <sheet name="calculate" sheetId="8" r:id="rId2"/>
+    <sheet name="by-name" sheetId="7" r:id="rId3"/>
+    <sheet name="ALL_uncontested" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="196">
   <si>
     <t>year</t>
   </si>
@@ -542,13 +543,88 @@
   </si>
   <si>
     <t>num_uncont</t>
+  </si>
+  <si>
+    <t>SENATE % uncontested</t>
+  </si>
+  <si>
+    <t>HOUSE % uncontested</t>
+  </si>
+  <si>
+    <t>TOTAL uncontested</t>
+  </si>
+  <si>
+    <t>total seats</t>
+  </si>
+  <si>
+    <t>^^ HOUSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOUSE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># indiv uncont &gt;= 3 in house: </t>
+  </si>
+  <si>
+    <t>Clark Jenkins</t>
+  </si>
+  <si>
+    <t>Daniel G. Clodfelter</t>
+  </si>
+  <si>
+    <t>Harry Brown</t>
+  </si>
+  <si>
+    <t>Jerry W. Tillman</t>
+  </si>
+  <si>
+    <t>Katie G. Dorsett</t>
+  </si>
+  <si>
+    <t>Linda Garrou</t>
+  </si>
+  <si>
+    <t>Peter Samuel (Pete) Brunstetter</t>
+  </si>
+  <si>
+    <t>Philip E. (Phil) Berger</t>
+  </si>
+  <si>
+    <t>Tom Apodaca</t>
+  </si>
+  <si>
+    <t>Tony Rand</t>
+  </si>
+  <si>
+    <t>David F. Weinstein</t>
+  </si>
+  <si>
+    <t>Austin Allran</t>
+  </si>
+  <si>
+    <t>Charlie Dannelly</t>
+  </si>
+  <si>
+    <t>James (Jim) Forrester</t>
+  </si>
+  <si>
+    <t>Stan Bingham</t>
+  </si>
+  <si>
+    <t>SENATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># indiv uncont &gt;=3 in senate: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># indiv uncont &gt;= 3 in NCGA: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -575,6 +651,25 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -656,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -675,6 +770,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9566,10 +9673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I12"/>
+  <dimension ref="A3:O12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="83" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="M13" sqref="M12:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9580,7 +9687,7 @@
     <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>168</v>
       </c>
@@ -9599,8 +9706,12 @@
       <c r="I3" s="9" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L3" s="12"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>163</v>
       </c>
@@ -9625,8 +9736,12 @@
       <c r="I4" s="6">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -9651,8 +9766,12 @@
       <c r="I5" s="6">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2002</v>
       </c>
@@ -9677,8 +9796,12 @@
       <c r="I6" s="6">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2004</v>
       </c>
@@ -9703,8 +9826,12 @@
       <c r="I7" s="6">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2006</v>
       </c>
@@ -9729,8 +9856,12 @@
       <c r="I8" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2008</v>
       </c>
@@ -9755,8 +9886,12 @@
       <c r="I9" s="6">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+    </row>
+    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2010</v>
       </c>
@@ -9781,8 +9916,12 @@
       <c r="I10" s="6">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+    </row>
+    <row r="11" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2012</v>
       </c>
@@ -9808,7 +9947,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>164</v>
       </c>
@@ -9830,10 +9969,1086 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="6">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6">
+        <v>31</v>
+      </c>
+      <c r="E2" s="19">
+        <v>120</v>
+      </c>
+      <c r="G2" s="14">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="15">
+        <v>6</v>
+      </c>
+      <c r="I2" s="15">
+        <v>4</v>
+      </c>
+      <c r="J2" s="15">
+        <v>10</v>
+      </c>
+      <c r="K2" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2002</v>
+      </c>
+      <c r="B3" s="6">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>27</v>
+      </c>
+      <c r="E3" s="19">
+        <v>120</v>
+      </c>
+      <c r="G3" s="14">
+        <v>2002</v>
+      </c>
+      <c r="H3" s="15">
+        <v>4</v>
+      </c>
+      <c r="I3" s="15">
+        <v>3</v>
+      </c>
+      <c r="J3" s="15">
+        <v>7</v>
+      </c>
+      <c r="K3" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>2004</v>
+      </c>
+      <c r="B4" s="6">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6">
+        <v>55</v>
+      </c>
+      <c r="E4" s="19">
+        <v>120</v>
+      </c>
+      <c r="G4" s="14">
+        <v>2004</v>
+      </c>
+      <c r="H4" s="15">
+        <v>6</v>
+      </c>
+      <c r="I4" s="15">
+        <v>5</v>
+      </c>
+      <c r="J4" s="15">
+        <v>11</v>
+      </c>
+      <c r="K4" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2006</v>
+      </c>
+      <c r="B5" s="6">
+        <v>32</v>
+      </c>
+      <c r="C5" s="6">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6">
+        <v>63</v>
+      </c>
+      <c r="E5" s="19">
+        <v>120</v>
+      </c>
+      <c r="G5" s="14">
+        <v>2006</v>
+      </c>
+      <c r="H5" s="15">
+        <v>12</v>
+      </c>
+      <c r="I5" s="15">
+        <v>10</v>
+      </c>
+      <c r="J5" s="15">
+        <v>22</v>
+      </c>
+      <c r="K5" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>2008</v>
+      </c>
+      <c r="B6" s="6">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6">
+        <v>50</v>
+      </c>
+      <c r="E6" s="19">
+        <v>120</v>
+      </c>
+      <c r="G6" s="14">
+        <v>2008</v>
+      </c>
+      <c r="H6" s="15">
+        <v>10</v>
+      </c>
+      <c r="I6" s="15">
+        <v>10</v>
+      </c>
+      <c r="J6" s="15">
+        <v>20</v>
+      </c>
+      <c r="K6" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>2010</v>
+      </c>
+      <c r="B7" s="6">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6">
+        <v>29</v>
+      </c>
+      <c r="D7" s="6">
+        <v>40</v>
+      </c>
+      <c r="E7" s="19">
+        <v>120</v>
+      </c>
+      <c r="G7" s="14">
+        <v>2010</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1</v>
+      </c>
+      <c r="I7" s="15">
+        <v>11</v>
+      </c>
+      <c r="J7" s="15">
+        <v>12</v>
+      </c>
+      <c r="K7" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2012</v>
+      </c>
+      <c r="B8" s="6">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6">
+        <v>49</v>
+      </c>
+      <c r="E8" s="19">
+        <v>120</v>
+      </c>
+      <c r="G8" s="14">
+        <v>2012</v>
+      </c>
+      <c r="H8" s="15">
+        <v>7</v>
+      </c>
+      <c r="I8" s="15">
+        <v>11</v>
+      </c>
+      <c r="J8" s="15">
+        <v>18</v>
+      </c>
+      <c r="K8" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="7">
+        <v>156</v>
+      </c>
+      <c r="C9" s="7">
+        <v>159</v>
+      </c>
+      <c r="D9" s="7">
+        <v>315</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E2:E8)</f>
+        <v>840</v>
+      </c>
+      <c r="J9">
+        <f>SUM(J2:J8)</f>
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <f>SUM(K2:K8)</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D12" s="3">
+        <v>2000</v>
+      </c>
+      <c r="E12" s="6">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6">
+        <v>14</v>
+      </c>
+      <c r="G12" s="6">
+        <v>31</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12">
+        <f>J9/K9</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J12">
+        <f>D9/E9</f>
+        <v>0.375</v>
+      </c>
+      <c r="K12">
+        <f>(J9+D9)/(E9+K9)</f>
+        <v>0.34873949579831931</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D13" s="3">
+        <v>2002</v>
+      </c>
+      <c r="E13" s="6">
+        <v>15</v>
+      </c>
+      <c r="F13" s="6">
+        <v>12</v>
+      </c>
+      <c r="G13" s="6">
+        <v>27</v>
+      </c>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="3">
+        <v>2004</v>
+      </c>
+      <c r="E14" s="6">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6">
+        <v>28</v>
+      </c>
+      <c r="G14" s="6">
+        <v>55</v>
+      </c>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D15" s="3">
+        <v>2006</v>
+      </c>
+      <c r="E15" s="6">
+        <v>32</v>
+      </c>
+      <c r="F15" s="6">
+        <v>31</v>
+      </c>
+      <c r="G15" s="6">
+        <v>63</v>
+      </c>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D16" s="3">
+        <v>2008</v>
+      </c>
+      <c r="E16" s="6">
+        <v>30</v>
+      </c>
+      <c r="F16" s="6">
+        <v>20</v>
+      </c>
+      <c r="G16" s="6">
+        <v>50</v>
+      </c>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D17" s="3">
+        <v>2010</v>
+      </c>
+      <c r="E17" s="6">
+        <v>11</v>
+      </c>
+      <c r="F17" s="6">
+        <v>29</v>
+      </c>
+      <c r="G17" s="6">
+        <v>40</v>
+      </c>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D18" s="3">
+        <v>2012</v>
+      </c>
+      <c r="E18" s="6">
+        <v>24</v>
+      </c>
+      <c r="F18" s="6">
+        <v>25</v>
+      </c>
+      <c r="G18" s="6">
+        <v>49</v>
+      </c>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D19" s="14">
+        <v>2000</v>
+      </c>
+      <c r="E19" s="15">
+        <v>6</v>
+      </c>
+      <c r="F19" s="15">
+        <v>4</v>
+      </c>
+      <c r="G19" s="15">
+        <v>10</v>
+      </c>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D20" s="14">
+        <v>2002</v>
+      </c>
+      <c r="E20" s="15">
+        <v>4</v>
+      </c>
+      <c r="F20" s="15">
+        <v>3</v>
+      </c>
+      <c r="G20" s="15">
+        <v>7</v>
+      </c>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D21" s="14">
+        <v>2004</v>
+      </c>
+      <c r="E21" s="15">
+        <v>6</v>
+      </c>
+      <c r="F21" s="15">
+        <v>5</v>
+      </c>
+      <c r="G21" s="15">
+        <v>11</v>
+      </c>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D22" s="14">
+        <v>2006</v>
+      </c>
+      <c r="E22" s="15">
+        <v>12</v>
+      </c>
+      <c r="F22" s="15">
+        <v>10</v>
+      </c>
+      <c r="G22" s="15">
+        <v>22</v>
+      </c>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D23" s="14">
+        <v>2008</v>
+      </c>
+      <c r="E23" s="15">
+        <v>10</v>
+      </c>
+      <c r="F23" s="15">
+        <v>10</v>
+      </c>
+      <c r="G23" s="15">
+        <v>20</v>
+      </c>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D24" s="14">
+        <v>2010</v>
+      </c>
+      <c r="E24" s="15">
+        <v>1</v>
+      </c>
+      <c r="F24" s="15">
+        <v>11</v>
+      </c>
+      <c r="G24" s="15">
+        <v>12</v>
+      </c>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D25" s="14">
+        <v>2012</v>
+      </c>
+      <c r="E25" s="15">
+        <v>7</v>
+      </c>
+      <c r="F25" s="15">
+        <v>11</v>
+      </c>
+      <c r="G25" s="15">
+        <v>18</v>
+      </c>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <f>SUM(E12:E25)</f>
+        <v>202</v>
+      </c>
+      <c r="F26">
+        <f>SUM(F12:F25)</f>
+        <v>213</v>
+      </c>
+      <c r="G26">
+        <f>SUM(G12:G25)</f>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28">
+        <f>COUNT(B29:B75)</f>
+        <v>47</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="6">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29">
+        <f>COUNT(H30:H44)</f>
+        <v>15</v>
+      </c>
+      <c r="G29" t="s">
+        <v>169</v>
+      </c>
+      <c r="H29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="6">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>195</v>
+      </c>
+      <c r="E30">
+        <f>SUM(E28:E29)</f>
+        <v>62</v>
+      </c>
+      <c r="G30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="6">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="6">
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>180</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="6">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3</v>
+      </c>
+      <c r="G34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="6">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>183</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="6">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>184</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="6">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>185</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="6">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>186</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="6">
+        <v>3</v>
+      </c>
+      <c r="G39" t="s">
+        <v>187</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="6">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
+        <v>188</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="6">
+        <v>3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>189</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="6">
+        <v>3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>190</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="6">
+        <v>3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>191</v>
+      </c>
+      <c r="H43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="6">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>192</v>
+      </c>
+      <c r="H44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B71" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView topLeftCell="E151" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116:K162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -13496,12 +14711,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>